<commit_message>
Updated to now parse controller commands from a connected xbox client
And some touchups to comments
</commit_message>
<xml_diff>
--- a/doc/bom.xlsx
+++ b/doc/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Github\Mini-Arm\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF27553-A152-4B2D-986C-638850AAACCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9C7D24-C1CE-4BA6-8A4A-48837568C477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{1D8C335D-01BB-457B-BD2C-7FAEE48B311C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{1D8C335D-01BB-457B-BD2C-7FAEE48B311C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Part</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Resistors</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A3D217-5318-4CCC-B9DB-49920EF49187}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -624,6 +627,15 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15" s="2"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <f>SUM(B2:B24)</f>
+        <v>44.1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>